<commit_message>
24 01 2024 v1.0
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Notes.xlsx
+++ b/src/main/resources/templates/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Worspace\pilpose\pilpose-back\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4AEF1A-53D8-4130-9DA7-8CAC6C0FA7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5950359F-0B09-456D-96FA-2F3D3AB60AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Référence</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Date de note</t>
+  </si>
+  <si>
+    <t>Statut</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,9 +395,10 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -407,6 +411,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>